<commit_message>
Pilgrimage, Purification and Saga images
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504CD45B-67FB-4F37-A02D-8EE01D83A1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509965D4-7951-41D9-992C-45E101B31BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -798,7 +798,7 @@
   <dimension ref="A1:E300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Cloning, Void and WarTactics images
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509965D4-7951-41D9-992C-45E101B31BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9CD86F-2F44-4873-946D-E695F924AA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1256,7 +1256,7 @@
         <v>55</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1282,7 +1282,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1369,7 +1369,7 @@
         <v>55</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>

</xml_diff>

<commit_message>
Avarice, BloodyArmor, BloodyStrike images
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9CD86F-2F44-4873-946D-E695F924AA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589735E7-62EC-4167-9435-A85B8866C7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -861,7 +861,7 @@
         <v>56</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -913,7 +913,7 @@
         <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -926,7 +926,7 @@
         <v>55</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -965,7 +965,7 @@
         <v>55</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1460,7 +1460,7 @@
         <v>55</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1473,7 +1473,7 @@
         <v>55</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>

</xml_diff>

<commit_message>
Feast, Injury and LeaveItToFate images
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589735E7-62EC-4167-9435-A85B8866C7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A096E8FE-95E2-4350-BA17-9986CCD4D444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1108,7 +1108,7 @@
         <v>55</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1191,7 +1191,7 @@
         <v>55</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1204,7 +1204,7 @@
         <v>56</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>

</xml_diff>

<commit_message>
add ExecutionStrike. ColdBlood, Frenzy and SpikyDefend images
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A096E8FE-95E2-4350-BA17-9986CCD4D444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675BE13E-1259-47AB-8EB0-F16AE9400207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add ArmyOfSoldiers, tokens related and exclude them for the card pool
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675BE13E-1259-47AB-8EB0-F16AE9400207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF07D75A-697C-412D-A569-55F16436A3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -978,7 +978,7 @@
         <v>55</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1121,7 +1121,7 @@
         <v>55</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1382,7 +1382,7 @@
         <v>55</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>

</xml_diff>

<commit_message>
Exposure, CommandingPresence and Unsheathe images + small fixs
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF07D75A-697C-412D-A569-55F16436A3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C2B1DA-56D6-4CA5-82AD-B1D32D0527F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="60">
   <si>
     <t>AllInOne</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>DESC (+ UPG)</t>
+  </si>
+  <si>
+    <t>ArmyOfSoldiers</t>
+  </si>
+  <si>
+    <t>CommandingPresence</t>
   </si>
 </sst>
 </file>
@@ -797,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1082,7 +1088,7 @@
         <v>55</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1447,7 +1453,7 @@
         <v>55</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1486,16 +1492,28 @@
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="A54" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="A55" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
     </row>

</xml_diff>

<commit_message>
ArmyOfSoldiers, Hustle, Replenishment and StrategicStrikes images
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C2B1DA-56D6-4CA5-82AD-B1D32D0527F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101C123A-C9D7-4070-9275-03D1B4206DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ListOfCards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1184,7 +1184,7 @@
         <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1336,7 +1336,7 @@
         <v>56</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1401,7 +1401,7 @@
         <v>55</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1499,7 +1499,7 @@
         <v>55</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1512,7 +1512,7 @@
         <v>55</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>

</xml_diff>

<commit_message>
Add Ambush, Catharsis, MobileFortress,ClumsyStrike and some images.
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101C123A-C9D7-4070-9275-03D1B4206DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C396C90-5304-482F-9C99-5593A9C73FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>AllInOne</t>
   </si>
@@ -200,6 +200,24 @@
   </si>
   <si>
     <t>CommandingPresence</t>
+  </si>
+  <si>
+    <t>ExecutionStrike</t>
+  </si>
+  <si>
+    <t>FirstStrike</t>
+  </si>
+  <si>
+    <t>MobileFortress</t>
+  </si>
+  <si>
+    <t>Catharsis</t>
+  </si>
+  <si>
+    <t>Ambush</t>
+  </si>
+  <si>
+    <t>ClumsyStrike</t>
   </si>
 </sst>
 </file>
@@ -804,7 +822,7 @@
   <dimension ref="A1:E300"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1440,7 +1458,7 @@
         <v>55</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1518,44 +1536,80 @@
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="A56" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="A57" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="A58" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="A59" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="A60" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="A61" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
     </row>

</xml_diff>

<commit_message>
Add BulwarkOfTheTitan, RejuvenatingBreath WIP and MobileFortress and FirstStrike images
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C396C90-5304-482F-9C99-5593A9C73FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461EB774-CB47-438F-A65E-14F69E0DE007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="67">
   <si>
     <t>AllInOne</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>ClumsyStrike</t>
+  </si>
+  <si>
+    <t>BulwarkOfTheTitan</t>
   </si>
 </sst>
 </file>
@@ -821,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -1614,9 +1617,15 @@
       <c r="E61" s="2"/>
     </row>
     <row r="62" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="A62" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
     </row>

</xml_diff>

<commit_message>
Add Catharsis, ClumsyStrike and FacingDestiny images
</commit_message>
<xml_diff>
--- a/ListOfCards.xlsx
+++ b/ListOfCards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlowUP\IdeaProjects\BloodElfModForSlayTheSpire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461EB774-CB47-438F-A65E-14F69E0DE007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826BC85F-1011-4885-AF55-88C5A06763F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfCards" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>AllInOne</t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>RealStrength</t>
-  </si>
-  <si>
-    <t>Redemption</t>
   </si>
   <si>
     <t>Replenishment</t>
@@ -824,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -839,19 +836,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
@@ -859,10 +856,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -872,10 +869,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -885,10 +882,10 @@
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -898,10 +895,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -911,10 +908,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -924,10 +921,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -937,10 +934,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -950,10 +947,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -963,10 +960,10 @@
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -976,10 +973,10 @@
         <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -989,10 +986,10 @@
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1002,10 +999,10 @@
         <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1015,10 +1012,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1028,10 +1025,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1041,10 +1038,10 @@
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1054,10 +1051,10 @@
         <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1067,10 +1064,10 @@
         <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1080,10 +1077,10 @@
         <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1093,10 +1090,10 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1106,10 +1103,10 @@
         <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1119,10 +1116,10 @@
         <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1132,10 +1129,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1145,10 +1142,10 @@
         <v>33</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1158,10 +1155,10 @@
         <v>34</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1180,10 +1177,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1202,10 +1199,10 @@
         <v>36</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1215,10 +1212,10 @@
         <v>37</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1228,10 +1225,10 @@
         <v>38</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1241,10 +1238,10 @@
         <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1254,10 +1251,10 @@
         <v>16</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1267,10 +1264,10 @@
         <v>39</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1280,10 +1277,10 @@
         <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1293,10 +1290,10 @@
         <v>41</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1306,10 +1303,10 @@
         <v>42</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1324,15 +1321,9 @@
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
-      <c r="A39" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
@@ -1341,23 +1332,23 @@
         <v>17</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A41" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1367,10 +1358,10 @@
         <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1380,36 +1371,36 @@
         <v>11</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1419,10 +1410,10 @@
         <v>18</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1432,10 +1423,10 @@
         <v>12</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1445,36 +1436,36 @@
         <v>19</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A49" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A50" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1484,23 +1475,23 @@
         <v>13</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1514,117 +1505,117 @@
     </row>
     <row r="54" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A54" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A55" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A56" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A57" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A58" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A59" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A60" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A61" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
     </row>
     <row r="62" spans="1:5" ht="21.5" x14ac:dyDescent="0.75">
       <c r="A62" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>

</xml_diff>